<commit_message>
Shrink beam pipe to 3.5cm radius and add log scale to energy in plotprogression
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-LsrDrvn-Solenoid.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-LsrDrvn-Solenoid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFD1584-3938-A943-BAB1-C9B8F1A748FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C1F242-DC8A-644B-B199-806F124A94B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6040" yWindow="640" windowWidth="21660" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -843,7 +843,7 @@
   <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,7 +947,7 @@
         <v>66</v>
       </c>
       <c r="F4" s="9">
-        <v>0.5</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>14</v>

</xml_diff>